<commit_message>
Unit tests and Refactoring
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BED531E-2B5A-4364-B906-9B7CCE1D4930}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3873B41B-EA22-4A44-8DF6-78BAC383E185}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="69720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult Funding Claim" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Provider :</t>
   </si>
@@ -37,15 +37,6 @@
     <t>ILR File :</t>
   </si>
   <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Main Body</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>OFFICIAL - SENSITIVE</t>
   </si>
   <si>
@@ -61,16 +52,10 @@
     <t>Postcode Data:</t>
   </si>
   <si>
-    <t>Footer</t>
-  </si>
-  <si>
     <t>Advanced Learner Loans Bursary</t>
   </si>
   <si>
     <t>Adult Funding Claim Report</t>
-  </si>
-  <si>
-    <t>This report displays indicative figures only.</t>
   </si>
   <si>
     <t>Actual earnings 
@@ -83,45 +68,6 @@
 - year-end claims</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This note is to be displayed </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>only</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> on the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>FIS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> version of the report</t>
-    </r>
-  </si>
-  <si>
     <t>Actual earnings 
 (12 months)
 - final claims</t>
@@ -136,30 +82,6 @@
     <t>Excess Support</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Total </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Advanced Learner</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Loans Bursary Delivery</t>
-    </r>
-  </si>
-  <si>
     <t>Last ILR File Update:</t>
   </si>
   <si>
@@ -169,191 +91,12 @@
     <t>Campus Id Data:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ESFA </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Adult Education Budget - Non-procured</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Total</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ESFA </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Adult Education Budget - Non-procured</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Delivery</t>
-    </r>
-  </si>
-  <si>
     <t>ESFA AEB Adult Skills - programme funding</t>
   </si>
   <si>
     <t>ESFA AEB Adult Skills - learning support</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ESFA AEB </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">19-24 Traineeships - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">rogramme </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>unding</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ESFA AEB</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 19-24 Traineeships - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>l</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">earning </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>upport</t>
-    </r>
-  </si>
-  <si>
     <t>Year:</t>
   </si>
   <si>
@@ -448,6 +191,30 @@
   </si>
   <si>
     <t>&amp;=AdultFundingClaim.ALBExcessSupport.FinalClaims</t>
+  </si>
+  <si>
+    <t>ESFA Adult Education Budget - Non-procured</t>
+  </si>
+  <si>
+    <t>ESFA AEB 19-24 Traineeships - programme funding</t>
+  </si>
+  <si>
+    <t>ESFA AEB 19-24 Traineeships - learning support</t>
+  </si>
+  <si>
+    <t>Total ESFA Adult Education Budget - Non-procured Delivery</t>
+  </si>
+  <si>
+    <t>Total Advanced Learner Loans Bursary Delivery</t>
+  </si>
+  <si>
+    <t>&amp;=AdultFundingClaim.LastEASFileUpdate</t>
+  </si>
+  <si>
+    <t>&amp;=AdultFundingClaim.LastILRFileUpdate</t>
+  </si>
+  <si>
+    <t>This report displays indicative figures only.</t>
   </si>
 </sst>
 </file>
@@ -459,7 +226,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -470,19 +237,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF00B050"/>
       <name val="Arial"/>
@@ -523,24 +277,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,18 +302,6 @@
         <bgColor indexed="0"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -718,9 +449,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -729,7 +460,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -738,23 +469,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -762,27 +493,27 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
@@ -803,30 +534,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
@@ -840,59 +571,20 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -986,9 +678,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
+      <xdr:colOff>47624</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="8439151" cy="1443038"/>
     <xdr:sp macro="" textlink="">
@@ -1004,7 +696,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="538162" y="6786562"/>
+          <a:off x="257174" y="6153149"/>
           <a:ext cx="8439151" cy="1443038"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1036,20 +728,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="900">
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="900">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>)     This report is intended for providers who are paid on profile to</a:t>
+            <a:t>1)     This report is intended for providers who are paid on profile to</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="900" baseline="0">
@@ -1059,47 +744,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> assist them in preparing for mid-year </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="900" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>forecast</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="900" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>, year-end </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="900" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>forecast</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="900" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> and final-year claims</a:t>
+            <a:t> assist them in preparing for mid-year forecast, year-end forecast and final-year claims</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="900">
             <a:solidFill>
@@ -1122,7 +767,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="900">
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
@@ -1132,7 +777,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="900" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
@@ -1141,7 +786,7 @@
           </a:r>
           <a:endParaRPr lang="en-GB" sz="900">
             <a:solidFill>
-              <a:srgbClr val="00B050"/>
+              <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
             <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
@@ -1184,18 +829,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>3)     </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Devolved adult education funding for learners who are funded through the Mayoral Combined Authorities or Greater London Authority is not included in this report</a:t>
+            <a:t>3)     Devolved adult education funding for learners who are funded through the Mayoral Combined Authorities or Greater London Authority is not included in this report</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1218,7 +852,7 @@
           </a:pPr>
           <a:endParaRPr lang="en-GB" sz="900">
             <a:solidFill>
-              <a:srgbClr val="00B050"/>
+              <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
             <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
             <a:ea typeface="+mn-ea"/>
@@ -1246,7 +880,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="900">
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
@@ -1257,7 +891,7 @@
           <a:r>
             <a:rPr lang="en-GB" sz="900" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
@@ -1274,18 +908,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>The Discretionary Learner Support elements of the Advanced Learner Loans Bursary (Hardship, Childcare and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="900">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Residential Access Fund) are not included as these are not earned through the ILR or EAS</a:t>
+            <a:t>The Discretionary Learner Support elements of the Advanced Learner Loans Bursary (Hardship, Childcare and Residential Access Fund) are not included as these are not earned through the ILR or EAS</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1662,27 +1285,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:Q43"/>
+  <dimension ref="B2:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19" style="5" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="5" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="5" customWidth="1"/>
     <col min="6" max="8" width="20.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" style="5" customWidth="1"/>
     <col min="10" max="10" width="2.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="5"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1691,29 +1313,25 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
-      <c r="K2" s="48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" ht="20.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:12" ht="20.25" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
+      <c r="F3" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="40"/>
+      <c r="K3" s="10"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="6"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1722,15 +1340,14 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
-      <c r="K4" s="40"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="6"/>
       <c r="C5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>33</v>
+      <c r="D5" s="36" t="s">
+        <v>22</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="11"/>
@@ -1738,15 +1355,14 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
-      <c r="K5" s="40"/>
-    </row>
-    <row r="6" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>34</v>
+      <c r="D6" s="36" t="s">
+        <v>23</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="11"/>
@@ -1754,29 +1370,27 @@
       <c r="H6" s="8"/>
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="40"/>
-    </row>
-    <row r="7" spans="2:17" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="6"/>
       <c r="C7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="37" t="s">
-        <v>35</v>
+      <c r="D7" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="37" t="s">
-        <v>36</v>
+      <c r="G7" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>25</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="40"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -1785,32 +1399,20 @@
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="12"/>
-      <c r="K8" s="41"/>
-    </row>
-    <row r="9" spans="2:17" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
-      <c r="C9" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
+      <c r="C9" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
       <c r="I9" s="12"/>
-      <c r="K9" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="50"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1819,112 +1421,106 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="12"/>
-      <c r="K10" s="52"/>
-    </row>
-    <row r="11" spans="2:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
-      <c r="C11" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
+      <c r="C11" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I11" s="12"/>
-      <c r="K11" s="52"/>
-    </row>
-    <row r="12" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="42" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="44"/>
       <c r="F12" s="19" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="I12" s="12"/>
-      <c r="K12" s="52"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-    </row>
-    <row r="13" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="42" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="44"/>
       <c r="F13" s="19" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="I13" s="12"/>
-      <c r="K13" s="52"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-    </row>
-    <row r="14" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
-      <c r="C14" s="45" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="47"/>
+      <c r="C14" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="19" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="K14" s="52"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-    </row>
-    <row r="15" spans="2:17" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6"/>
-      <c r="C15" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="47"/>
+      <c r="C15" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="19" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="I15" s="12"/>
-      <c r="K15" s="52"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="6"/>
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
@@ -1933,14 +1529,13 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="12"/>
-      <c r="K16" s="52"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="6"/>
       <c r="C17" s="42" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="44"/>
@@ -1957,9 +1552,8 @@
         <v>0</v>
       </c>
       <c r="I17" s="12"/>
-      <c r="K17" s="52"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="6"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1968,85 +1562,80 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="12"/>
-      <c r="K18" s="52"/>
-    </row>
-    <row r="19" spans="2:13" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6"/>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="57"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="I19" s="12"/>
-      <c r="K19" s="52"/>
-    </row>
-    <row r="20" spans="2:13" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B20" s="6"/>
       <c r="C20" s="42" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="44"/>
       <c r="F20" s="19" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I20" s="12"/>
-      <c r="K20" s="52"/>
-    </row>
-    <row r="21" spans="2:13" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B21" s="6"/>
       <c r="C21" s="42" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D21" s="43"/>
       <c r="E21" s="44"/>
       <c r="F21" s="19" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="I21" s="12"/>
-      <c r="K21" s="52"/>
-    </row>
-    <row r="22" spans="2:13" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B22" s="6"/>
       <c r="C22" s="42" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D22" s="43"/>
       <c r="E22" s="44"/>
       <c r="F22" s="19" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="I22" s="12"/>
-      <c r="K22" s="52"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="6"/>
       <c r="C23" s="21"/>
       <c r="D23" s="24"/>
@@ -2055,17 +1644,16 @@
       <c r="G23" s="26"/>
       <c r="H23" s="26"/>
       <c r="I23" s="12"/>
-      <c r="K23" s="52"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="6"/>
-      <c r="C24" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="47"/>
+      <c r="C24" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="23">
         <f>SUM(F20:F22)</f>
         <v>0</v>
@@ -2079,9 +1667,8 @@
         <v>0</v>
       </c>
       <c r="I24" s="12"/>
-      <c r="K24" s="52"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="6"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -2090,9 +1677,8 @@
       <c r="G25" s="17"/>
       <c r="H25" s="17"/>
       <c r="I25" s="12"/>
-      <c r="K25" s="53"/>
-    </row>
-    <row r="26" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="6"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2101,11 +1687,8 @@
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="12"/>
-      <c r="K26" s="48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="6"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -2114,9 +1697,8 @@
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="12"/>
-      <c r="K27" s="40"/>
-    </row>
-    <row r="28" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="6"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -2125,9 +1707,8 @@
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="12"/>
-      <c r="K28" s="40"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="6"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -2136,9 +1717,8 @@
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="12"/>
-      <c r="K29" s="40"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="6"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -2147,9 +1727,8 @@
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="12"/>
-      <c r="K30" s="40"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
@@ -2158,9 +1737,8 @@
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
       <c r="I31" s="12"/>
-      <c r="K31" s="40"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" s="6"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -2169,9 +1747,8 @@
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
       <c r="I32" s="12"/>
-      <c r="K32" s="40"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="6"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -2180,9 +1757,8 @@
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="12"/>
-      <c r="K33" s="41"/>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="6"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -2191,9 +1767,8 @@
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="12"/>
-      <c r="K34" s="35"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="6"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -2202,9 +1777,8 @@
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="12"/>
-      <c r="K35" s="35"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="6"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -2213,9 +1787,8 @@
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="12"/>
-      <c r="K36" s="35"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="6"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2224,87 +1797,80 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="12"/>
-      <c r="K37" s="40" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="6"/>
       <c r="C38" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="39" t="s">
-        <v>41</v>
+        <v>6</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="E38" s="27"/>
       <c r="F38" s="27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G38" s="49" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H38" s="49"/>
       <c r="I38" s="28"/>
-      <c r="K38" s="40"/>
-    </row>
-    <row r="39" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="6"/>
       <c r="C39" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>41</v>
+        <v>16</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>59</v>
       </c>
       <c r="E39" s="29"/>
       <c r="F39" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" s="38"/>
+        <v>5</v>
+      </c>
+      <c r="G39" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="H39" s="37"/>
       <c r="I39" s="28"/>
-      <c r="K39" s="40"/>
-    </row>
-    <row r="40" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="6"/>
       <c r="C40" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>58</v>
       </c>
       <c r="F40" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="H40" s="38"/>
+        <v>7</v>
+      </c>
+      <c r="G40" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="37"/>
       <c r="I40" s="28"/>
       <c r="J40" s="27"/>
-      <c r="K40" s="40"/>
-    </row>
-    <row r="41" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41" s="6"/>
       <c r="C41" s="27"/>
       <c r="D41" s="27"/>
       <c r="E41" s="27"/>
       <c r="F41" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G41" s="38" t="s">
-        <v>40</v>
+        <v>18</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>29</v>
       </c>
       <c r="H41" s="27"/>
       <c r="I41" s="28"/>
       <c r="J41" s="27"/>
-      <c r="K41" s="40"/>
-    </row>
-    <row r="42" spans="2:11" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="6"/>
-      <c r="C42" s="38" t="s">
-        <v>42</v>
+      <c r="C42" s="37" t="s">
+        <v>31</v>
       </c>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
@@ -2313,9 +1879,8 @@
       <c r="H42" s="27"/>
       <c r="I42" s="30"/>
       <c r="J42" s="31"/>
-      <c r="K42" s="40"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="32"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
@@ -2324,15 +1889,15 @@
       <c r="G43" s="17"/>
       <c r="H43" s="17"/>
       <c r="I43" s="33"/>
-      <c r="K43" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="L9:Q9"/>
-    <mergeCell ref="K2:K8"/>
-    <mergeCell ref="K9:K25"/>
+  <mergeCells count="14">
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="G38:H38"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C9:H9"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C14:E14"/>
@@ -2340,16 +1905,10 @@
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="K37:K43"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="K26:K33"/>
-    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="C9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="G24:H24 F24" unlockedFormula="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
89045 - Fixing format of totals on Adult FC template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3873B41B-EA22-4A44-8DF6-78BAC383E185}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF32FDC-4431-46FE-8918-4018C8E8B00F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="69720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22836" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult Funding Claim" sheetId="3" r:id="rId1"/>
@@ -224,7 +224,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="&quot;£&quot;\ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ 0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -501,10 +501,6 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -547,18 +543,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -571,6 +555,21 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -583,8 +582,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="172" fontId="4" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1288,23 +1288,23 @@
   <dimension ref="B2:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.1171875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="5.703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="19" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="5" customWidth="1"/>
-    <col min="6" max="8" width="20.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="4.140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="2.28515625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="4" max="4" width="22.87890625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.5859375" style="5" customWidth="1"/>
+    <col min="6" max="8" width="20.703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="4.1171875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="2.29296875" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.1171875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1314,24 +1314,24 @@
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="2:12" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12" ht="20" x14ac:dyDescent="0.4">
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1341,12 +1341,12 @@
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B5" s="6"/>
       <c r="C5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="14"/>
@@ -1356,12 +1356,12 @@
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="35" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="15"/>
@@ -1371,26 +1371,26 @@
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
       <c r="C7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="35" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="35" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -1400,7 +1400,7 @@
       <c r="H8" s="17"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6"/>
       <c r="C9" s="48" t="s">
         <v>60</v>
@@ -1412,7 +1412,7 @@
       <c r="H9" s="48"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="6"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1422,7 +1422,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6"/>
       <c r="C11" s="45" t="s">
         <v>53</v>
@@ -1440,13 +1440,13 @@
       </c>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="6"/>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="44"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="19" t="s">
         <v>32</v>
       </c>
@@ -1460,13 +1460,13 @@
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="6"/>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="44"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="19" t="s">
         <v>33</v>
       </c>
@@ -1480,13 +1480,13 @@
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
     </row>
-    <row r="14" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="6"/>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="19" t="s">
         <v>34</v>
       </c>
@@ -1500,13 +1500,13 @@
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="2:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="6"/>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="44"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="19" t="s">
         <v>35</v>
       </c>
@@ -1520,40 +1520,40 @@
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B16" s="6"/>
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="34"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="12"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B17" s="6"/>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="23">
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="49">
         <f>SUM(F12:F15)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="49">
         <f>SUM(G12:G15)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="49">
         <f>SUM(H12:H15)</f>
         <v>0</v>
       </c>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B18" s="6"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1563,13 +1563,13 @@
       <c r="H18" s="11"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="6"/>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="18" t="s">
         <v>10</v>
       </c>
@@ -1581,13 +1581,13 @@
       </c>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B20" s="6"/>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="44"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="19" t="s">
         <v>36</v>
       </c>
@@ -1599,13 +1599,13 @@
       </c>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B21" s="6"/>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="43"/>
-      <c r="E21" s="44"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="19" t="s">
         <v>37</v>
       </c>
@@ -1617,13 +1617,13 @@
       </c>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B22" s="6"/>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="43"/>
-      <c r="E22" s="44"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="19" t="s">
         <v>38</v>
       </c>
@@ -1635,40 +1635,40 @@
       </c>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B23" s="6"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="12"/>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B24" s="6"/>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="23">
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="49">
         <f>SUM(F20:F22)</f>
         <v>0</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="49">
         <f>SUM(G20:G22)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="49">
         <f>SUM(H20:H22)</f>
         <v>0</v>
       </c>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B25" s="6"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -1678,7 +1678,7 @@
       <c r="H25" s="17"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="6"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -1688,7 +1688,7 @@
       <c r="H26" s="11"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B27" s="6"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -1698,7 +1698,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="6"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -1708,7 +1708,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B29" s="6"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -1718,7 +1718,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B30" s="6"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -1728,7 +1728,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B31" s="6"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
@@ -1738,7 +1738,7 @@
       <c r="H31" s="11"/>
       <c r="I31" s="12"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B32" s="6"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -1748,7 +1748,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="12"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B33" s="6"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -1758,7 +1758,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B34" s="6"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -1768,7 +1768,7 @@
       <c r="H34" s="11"/>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B35" s="6"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -1778,7 +1778,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B36" s="6"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -1788,7 +1788,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="12"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B37" s="6"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1798,105 +1798,100 @@
       <c r="H37" s="3"/>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="6"/>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27" t="s">
+      <c r="E38" s="26"/>
+      <c r="F38" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="49" t="s">
+      <c r="G38" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="49"/>
-      <c r="I38" s="28"/>
-    </row>
-    <row r="39" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H38" s="40"/>
+      <c r="I38" s="27"/>
+    </row>
+    <row r="39" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B39" s="6"/>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="27" t="s">
+      <c r="D39" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="27" t="s">
+      <c r="E39" s="28"/>
+      <c r="F39" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="G39" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="H39" s="37"/>
-      <c r="I39" s="28"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H39" s="36"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B40" s="6"/>
       <c r="C40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="D40" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="27" t="s">
+      <c r="F40" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="37" t="s">
+      <c r="G40" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="H40" s="37"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="27"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H40" s="36"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="26"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B41" s="6"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27" t="s">
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="37" t="s">
+      <c r="G41" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="H41" s="27"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="27"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H41" s="26"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="26"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B42" s="6"/>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="31"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="32"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="30"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B43" s="31"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
       <c r="H43" s="17"/>
-      <c r="I43" s="33"/>
+      <c r="I43" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="G38:H38"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C17:E17"/>
@@ -1906,11 +1901,16 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="G38:H38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G24:H24 F24" unlockedFormula="1"/>
+    <ignoredError sqref="G24:H24" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Acceptable Excel format found _-£* 0.00 for totals
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF32FDC-4431-46FE-8918-4018C8E8B00F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9E278C-302F-42C6-A96B-7FB5E31A159E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22836" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-405" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult Funding Claim" sheetId="3" r:id="rId1"/>
@@ -224,7 +224,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="&quot;£&quot;\ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ \ 0.00"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* 0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -543,6 +543,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -555,34 +567,22 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1288,7 +1288,7 @@
   <dimension ref="B2:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
@@ -1321,11 +1321,11 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -1402,14 +1402,14 @@
     </row>
     <row r="9" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6"/>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1424,11 +1424,11 @@
     </row>
     <row r="11" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6"/>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="47"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="18" t="s">
         <v>10</v>
       </c>
@@ -1442,11 +1442,11 @@
     </row>
     <row r="12" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="6"/>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="19" t="s">
         <v>32</v>
       </c>
@@ -1462,11 +1462,11 @@
     </row>
     <row r="13" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="6"/>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="19" t="s">
         <v>33</v>
       </c>
@@ -1482,11 +1482,11 @@
     </row>
     <row r="14" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="6"/>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
       <c r="F14" s="19" t="s">
         <v>34</v>
       </c>
@@ -1502,11 +1502,11 @@
     </row>
     <row r="15" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="6"/>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="19" t="s">
         <v>35</v>
       </c>
@@ -1534,11 +1534,11 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B17" s="6"/>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="49">
         <f>SUM(F12:F15)</f>
         <v>0</v>
@@ -1565,11 +1565,11 @@
     </row>
     <row r="19" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="6"/>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="44"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="18" t="s">
         <v>10</v>
       </c>
@@ -1583,11 +1583,11 @@
     </row>
     <row r="20" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B20" s="6"/>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="19" t="s">
         <v>36</v>
       </c>
@@ -1601,11 +1601,11 @@
     </row>
     <row r="21" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B21" s="6"/>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="19" t="s">
         <v>37</v>
       </c>
@@ -1619,11 +1619,11 @@
     </row>
     <row r="22" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B22" s="6"/>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="19" t="s">
         <v>38</v>
       </c>
@@ -1649,11 +1649,11 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B24" s="6"/>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="49">
         <f>SUM(F20:F22)</f>
         <v>0</v>
@@ -1810,10 +1810,10 @@
       <c r="F38" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="40" t="s">
+      <c r="G38" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="40"/>
+      <c r="H38" s="48"/>
       <c r="I38" s="27"/>
     </row>
     <row r="39" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1892,6 +1892,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="G38:H38"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C17:E17"/>
@@ -1901,11 +1906,6 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="G38:H38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Format of total fields updated to include commas
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9E278C-302F-42C6-A96B-7FB5E31A159E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD6552B-B2AD-4C81-B877-957E8EEB9A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-405" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult Funding Claim" sheetId="3" r:id="rId1"/>
@@ -224,7 +224,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* 0.00"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -543,18 +543,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -567,6 +555,21 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -578,9 +581,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1288,7 +1288,7 @@
   <dimension ref="B2:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
@@ -1321,11 +1321,11 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -1402,14 +1402,14 @@
     </row>
     <row r="9" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="6"/>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1424,11 +1424,11 @@
     </row>
     <row r="11" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6"/>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="18" t="s">
         <v>10</v>
       </c>
@@ -1442,11 +1442,11 @@
     </row>
     <row r="12" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="6"/>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="19" t="s">
         <v>32</v>
       </c>
@@ -1462,11 +1462,11 @@
     </row>
     <row r="13" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="6"/>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="19" t="s">
         <v>33</v>
       </c>
@@ -1482,11 +1482,11 @@
     </row>
     <row r="14" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="6"/>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="19" t="s">
         <v>34</v>
       </c>
@@ -1502,11 +1502,11 @@
     </row>
     <row r="15" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="6"/>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="19" t="s">
         <v>35</v>
       </c>
@@ -1534,11 +1534,11 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B17" s="6"/>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="49">
         <f>SUM(F12:F15)</f>
         <v>0</v>
@@ -1565,11 +1565,11 @@
     </row>
     <row r="19" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="6"/>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="18" t="s">
         <v>10</v>
       </c>
@@ -1583,11 +1583,11 @@
     </row>
     <row r="20" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B20" s="6"/>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="19" t="s">
         <v>36</v>
       </c>
@@ -1601,11 +1601,11 @@
     </row>
     <row r="21" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B21" s="6"/>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="19" t="s">
         <v>37</v>
       </c>
@@ -1619,11 +1619,11 @@
     </row>
     <row r="22" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B22" s="6"/>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="42"/>
-      <c r="E22" s="43"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="19" t="s">
         <v>38</v>
       </c>
@@ -1649,11 +1649,11 @@
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B24" s="6"/>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
       <c r="F24" s="49">
         <f>SUM(F20:F22)</f>
         <v>0</v>
@@ -1810,10 +1810,10 @@
       <c r="F38" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="48" t="s">
+      <c r="G38" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="48"/>
+      <c r="H38" s="40"/>
       <c r="I38" s="27"/>
     </row>
     <row r="39" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1892,11 +1892,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="G38:H38"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C17:E17"/>
@@ -1906,6 +1901,11 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="G38:H38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2021 Adult Funding Claim Report Rollover
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD6552B-B2AD-4C81-B877-957E8EEB9A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99C7349-40F2-4E77-AA26-4B800D314962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Adult Funding Claim" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Adult Funding Claim'!$B$2:$I$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Adult Funding Claim'!$B$2:$I$44</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -19,6 +19,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,15 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t>Provider :</t>
   </si>
   <si>
     <t>UKPRN :</t>
-  </si>
-  <si>
-    <t>ILR File :</t>
   </si>
   <si>
     <t>OFFICIAL - SENSITIVE</t>
@@ -82,12 +80,6 @@
     <t>Excess Support</t>
   </si>
   <si>
-    <t>Last ILR File Update:</t>
-  </si>
-  <si>
-    <t>Last EAS File Update:</t>
-  </si>
-  <si>
     <t>Campus Id Data:</t>
   </si>
   <si>
@@ -208,13 +200,16 @@
     <t>Total Advanced Learner Loans Bursary Delivery</t>
   </si>
   <si>
-    <t>&amp;=AdultFundingClaim.LastEASFileUpdate</t>
-  </si>
-  <si>
-    <t>&amp;=AdultFundingClaim.LastILRFileUpdate</t>
-  </si>
-  <si>
     <t>This report displays indicative figures only.</t>
+  </si>
+  <si>
+    <t>Last ILR File :</t>
+  </si>
+  <si>
+    <t>Last EAS File :</t>
+  </si>
+  <si>
+    <t>&amp;=AdultFundingClaim.EasFile</t>
   </si>
 </sst>
 </file>
@@ -224,7 +219,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;£&quot;* #,##0.00"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -543,6 +538,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -581,10 +580,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -679,7 +674,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="8439151" cy="1443038"/>
@@ -1285,11 +1280,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:L43"/>
+  <dimension ref="B2:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1317,15 +1310,15 @@
     <row r="3" spans="2:12" ht="20" x14ac:dyDescent="0.4">
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
+      <c r="F3" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -1347,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="11"/>
@@ -1362,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="11"/>
@@ -1374,107 +1367,102 @@
     <row r="7" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
       <c r="C7" s="13" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="16"/>
+        <v>21</v>
+      </c>
+      <c r="E7" s="15"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>25</v>
-      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B9" s="6"/>
-      <c r="C9" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="6"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="C10" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="6"/>
-      <c r="C11" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="18" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="6"/>
+      <c r="C12" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="H12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="6"/>
-      <c r="C12" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>46</v>
-      </c>
       <c r="I12" s="12"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
     </row>
     <row r="13" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="6"/>
-      <c r="C13" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
+      <c r="C13" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
       <c r="F13" s="19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I13" s="12"/>
       <c r="K13" s="20"/>
@@ -1482,19 +1470,19 @@
     </row>
     <row r="14" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="6"/>
-      <c r="C14" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
+      <c r="C14" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I14" s="12"/>
       <c r="K14" s="20"/>
@@ -1502,193 +1490,203 @@
     </row>
     <row r="15" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="6"/>
-      <c r="C15" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
+      <c r="C15" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I15" s="12"/>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="6"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="C16" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>46</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B17" s="6"/>
-      <c r="C17" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="49">
-        <f>SUM(F12:F15)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="49">
-        <f>SUM(G12:G15)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="49">
-        <f>SUM(H12:H15)</f>
-        <v>0</v>
-      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
       <c r="I17" s="12"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B18" s="6"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
+      <c r="C18" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="37">
+        <f>SUM(F13:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="37">
+        <f>SUM(G13:G16)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="37">
+        <f>SUM(H13:H16)</f>
+        <v>0</v>
+      </c>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B19" s="6"/>
-      <c r="C19" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="18" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="6"/>
+      <c r="C20" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="44"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="H20" s="18" t="s">
         <v>11</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="2:12" ht="38" x14ac:dyDescent="0.4">
-      <c r="B20" s="6"/>
-      <c r="C20" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>50</v>
       </c>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B21" s="6"/>
-      <c r="C21" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
+      <c r="C21" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B22" s="6"/>
-      <c r="C22" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
+      <c r="C22" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="39"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B23" s="6"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
+      <c r="C23" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="39"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="I23" s="12"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B24" s="6"/>
-      <c r="C24" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="49">
-        <f>SUM(F20:F22)</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="49">
-        <f>SUM(G20:G22)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="49">
-        <f>SUM(H20:H22)</f>
-        <v>0</v>
-      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
       <c r="I24" s="12"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B25" s="6"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
+      <c r="C25" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="39"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="37">
+        <f>SUM(F21:F23)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="37">
+        <f>SUM(G21:G23)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="37">
+        <f>SUM(H21:H23)</f>
+        <v>0</v>
+      </c>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B26" s="6"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="6"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -1698,7 +1696,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B28" s="6"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -1708,7 +1706,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="6"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -1790,127 +1788,128 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B37" s="6"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B38" s="6"/>
-      <c r="C38" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="H38" s="40"/>
-      <c r="I38" s="27"/>
-    </row>
-    <row r="39" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B39" s="6"/>
       <c r="C39" s="26" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="28"/>
+        <v>27</v>
+      </c>
+      <c r="E39" s="26"/>
       <c r="F39" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G39" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="36"/>
+        <v>3</v>
+      </c>
+      <c r="G39" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39" s="41"/>
       <c r="I39" s="27"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B40" s="6"/>
-      <c r="C40" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>58</v>
-      </c>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="28"/>
       <c r="F40" s="26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G40" s="36" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="27"/>
-      <c r="J40" s="26"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B41" s="6"/>
-      <c r="C41" s="26"/>
       <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
       <c r="F41" s="26" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G41" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="H41" s="26"/>
+        <v>25</v>
+      </c>
+      <c r="H41" s="36"/>
       <c r="I41" s="27"/>
       <c r="J41" s="26"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B42" s="6"/>
-      <c r="C42" s="36" t="s">
-        <v>31</v>
-      </c>
+      <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
+      <c r="F42" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="36" t="s">
+        <v>26</v>
+      </c>
       <c r="H42" s="26"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="26"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B43" s="31"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="32"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="30"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B44" s="31"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C16:E16"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C10:H10"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="G39:H39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G24:H24" unlockedFormula="1"/>
+    <ignoredError sqref="G25:H25" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes to support ILR and EAS file name retrieval for headers on Funding Reports
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99C7349-40F2-4E77-AA26-4B800D314962}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F49D7C-5C2F-4718-BA00-9295F14E43E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="-19860" windowWidth="12120" windowHeight="8565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult Funding Claim" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Adult Funding Claim'!$B$2:$I$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Adult Funding Claim'!$B$2:$I$46</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Provider :</t>
   </si>
@@ -203,13 +203,25 @@
     <t>This report displays indicative figures only.</t>
   </si>
   <si>
-    <t>Last ILR File :</t>
-  </si>
-  <si>
-    <t>Last EAS File :</t>
-  </si>
-  <si>
     <t>&amp;=AdultFundingClaim.EasFile</t>
+  </si>
+  <si>
+    <t>ILR File :</t>
+  </si>
+  <si>
+    <t>Last EAS File Update :</t>
+  </si>
+  <si>
+    <t>Last ILR File Update :</t>
+  </si>
+  <si>
+    <t>EAS File :</t>
+  </si>
+  <si>
+    <t>&amp;=AdultFundingClaim.LastIlrFileUpdate</t>
+  </si>
+  <si>
+    <t>&amp;=AdultFundingClaim.LastEasFileUpdate</t>
   </si>
 </sst>
 </file>
@@ -542,6 +554,18 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -554,32 +578,20 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -674,7 +686,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="8439151" cy="1443038"/>
@@ -1280,7 +1292,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:L44"/>
+  <dimension ref="B2:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1288,7 +1300,7 @@
   <cols>
     <col min="1" max="1" width="3.1171875" style="5" customWidth="1"/>
     <col min="2" max="2" width="5.703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.17578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="22.87890625" style="5" customWidth="1"/>
     <col min="5" max="5" width="15.5859375" style="5" customWidth="1"/>
     <col min="6" max="8" width="20.703125" style="5" customWidth="1"/>
@@ -1314,11 +1326,11 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -1367,7 +1379,7 @@
     <row r="7" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B7" s="6"/>
       <c r="C7" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7" s="35" t="s">
         <v>21</v>
@@ -1382,127 +1394,117 @@
     <row r="8" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
       <c r="C8" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="E8" s="15"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>22</v>
-      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="9"/>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B9" s="6"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B10" s="6"/>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B11" s="6"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="6"/>
+      <c r="C12" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="6"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="6"/>
-      <c r="C12" s="46" t="s">
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="6"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="6"/>
+      <c r="C14" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="18" t="s">
+      <c r="D14" s="46"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G14" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="6"/>
-      <c r="C13" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="12"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-    </row>
-    <row r="14" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="6"/>
-      <c r="C14" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>44</v>
-      </c>
       <c r="I14" s="12"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
     </row>
     <row r="15" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="6"/>
-      <c r="C15" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
+      <c r="C15" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I15" s="12"/>
       <c r="K15" s="20"/>
@@ -1510,203 +1512,223 @@
     </row>
     <row r="16" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="6"/>
-      <c r="C16" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40"/>
+      <c r="C16" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="43"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I16" s="12"/>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="6"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="C17" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="43"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>45</v>
+      </c>
       <c r="I17" s="12"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="6"/>
-      <c r="C18" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="37">
-        <f>SUM(F13:F16)</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="37">
-        <f>SUM(G13:G16)</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="37">
-        <f>SUM(H13:H16)</f>
-        <v>0</v>
+      <c r="C18" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="I18" s="12"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B19" s="6"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B20" s="6"/>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="43"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="37">
+        <f>SUM(F15:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="37">
+        <f>SUM(G15:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="37">
+        <f>SUM(H15:H18)</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B21" s="6"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="6"/>
+      <c r="C22" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="18" t="s">
+      <c r="D22" s="40"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G22" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H22" s="18" t="s">
         <v>11</v>
-      </c>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="2:12" ht="38" x14ac:dyDescent="0.4">
-      <c r="B21" s="6"/>
-      <c r="C21" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="2:12" ht="38" x14ac:dyDescent="0.4">
-      <c r="B22" s="6"/>
-      <c r="C22" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="2:12" ht="38" x14ac:dyDescent="0.4">
       <c r="B23" s="6"/>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="2:12" ht="38" x14ac:dyDescent="0.4">
+      <c r="B24" s="6"/>
+      <c r="C24" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="2:12" ht="38" x14ac:dyDescent="0.4">
+      <c r="B25" s="6"/>
+      <c r="C25" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="19" t="s">
+      <c r="D25" s="43"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G25" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H25" s="19" t="s">
         <v>49</v>
-      </c>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="6"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="12"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B25" s="6"/>
-      <c r="C25" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="37">
-        <f>SUM(F21:F23)</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="37">
-        <f>SUM(G21:G23)</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="37">
-        <f>SUM(H21:H23)</f>
-        <v>0</v>
       </c>
       <c r="I25" s="12"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B26" s="6"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B27" s="6"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
+      <c r="C27" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="43"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="37">
+        <f>SUM(F23:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="37">
+        <f>SUM(G23:G25)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="37">
+        <f>SUM(H23:H25)</f>
+        <v>0</v>
+      </c>
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B28" s="6"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="6"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -1726,7 +1748,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="6"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
@@ -1798,118 +1820,138 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B38" s="6"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B39" s="6"/>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="12"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B40" s="6"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="6"/>
+      <c r="C41" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D41" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26" t="s">
+      <c r="E41" s="26"/>
+      <c r="F41" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G39" s="41" t="s">
+      <c r="G41" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="41"/>
-      <c r="I39" s="27"/>
-    </row>
-    <row r="40" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="6"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="H40" s="36"/>
-      <c r="I40" s="27"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B41" s="6"/>
-      <c r="D41" s="26"/>
-      <c r="F41" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="H41" s="36"/>
+      <c r="H41" s="49"/>
       <c r="I41" s="27"/>
-      <c r="J41" s="26"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.4">
+    </row>
+    <row r="42" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" s="6"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
+      <c r="E42" s="28"/>
       <c r="F42" s="26" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G42" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="H42" s="26"/>
+        <v>24</v>
+      </c>
+      <c r="H42" s="36"/>
       <c r="I42" s="27"/>
-      <c r="J42" s="26"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B43" s="6"/>
-      <c r="C43" s="36" t="s">
+      <c r="D43" s="26"/>
+      <c r="F43" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" s="36"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="26"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B44" s="6"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H44" s="26"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="26"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B45" s="6"/>
+      <c r="C45" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="29"/>
-      <c r="J43" s="30"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B44" s="31"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="32"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="30"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B46" s="31"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="G41:H41"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G25:H25" unlockedFormula="1"/>
+    <ignoredError sqref="G27:H27" unlockedFormula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
100878 adjusted header alignment
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC2ACD0-4EFC-4DE3-93B2-B5F06ADFB833}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E294766-1697-4FC1-96C1-E6AE409A960A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2844" yWindow="2316" windowWidth="21600" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult Funding Claim" sheetId="3" r:id="rId1"/>
@@ -13,13 +13,15 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Adult Funding Claim'!$B$2:$I$46</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -554,18 +556,6 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -578,6 +568,21 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -589,9 +594,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1294,22 +1296,24 @@
   </sheetPr>
   <dimension ref="B2:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.1328125" style="5" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.86328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="34" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.53125" style="5" customWidth="1"/>
     <col min="6" max="8" width="20.6640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="4.109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="4.1328125" style="5" customWidth="1"/>
     <col min="10" max="10" width="2.33203125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="5"/>
+    <col min="11" max="16384" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1319,24 +1323,24 @@
       <c r="H2" s="3"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="20.65" x14ac:dyDescent="0.35">
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="6"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1346,7 +1350,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
       <c r="C5" s="13" t="s">
         <v>0</v>
@@ -1361,7 +1365,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
       <c r="C6" s="13" t="s">
         <v>1</v>
@@ -1376,7 +1380,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B7" s="6"/>
       <c r="C7" s="13" t="s">
         <v>57</v>
@@ -1391,7 +1395,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B8" s="6"/>
       <c r="C8" s="13" t="s">
         <v>59</v>
@@ -1406,7 +1410,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B9" s="6"/>
       <c r="C9" s="13" t="s">
         <v>60</v>
@@ -1421,7 +1425,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B10" s="6"/>
       <c r="C10" s="13" t="s">
         <v>58</v>
@@ -1440,7 +1444,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="6"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -1450,19 +1454,19 @@
       <c r="H11" s="17"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -1472,13 +1476,13 @@
       <c r="H13" s="11"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="18" t="s">
         <v>9</v>
       </c>
@@ -1490,13 +1494,13 @@
       </c>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="44"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="19" t="s">
         <v>29</v>
       </c>
@@ -1510,13 +1514,13 @@
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
     </row>
-    <row r="16" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="44"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="40"/>
       <c r="F16" s="19" t="s">
         <v>30</v>
       </c>
@@ -1530,13 +1534,13 @@
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="44"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="19" t="s">
         <v>31</v>
       </c>
@@ -1550,13 +1554,13 @@
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
     </row>
-    <row r="18" spans="2:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="44"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="19" t="s">
         <v>32</v>
       </c>
@@ -1570,7 +1574,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B19" s="6"/>
       <c r="C19" s="21"/>
       <c r="D19" s="22"/>
@@ -1582,13 +1586,13 @@
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="44"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
       <c r="F20" s="37">
         <f>SUM(F15:F18)</f>
         <v>0</v>
@@ -1603,7 +1607,7 @@
       </c>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -1613,13 +1617,13 @@
       <c r="H21" s="11"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
-      <c r="C22" s="39" t="s">
+      <c r="C22" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45"/>
       <c r="F22" s="18" t="s">
         <v>9</v>
       </c>
@@ -1631,13 +1635,13 @@
       </c>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="2:12" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="38.25" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="44"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="19" t="s">
         <v>33</v>
       </c>
@@ -1649,13 +1653,13 @@
       </c>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="2:12" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="38.25" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="40"/>
       <c r="F24" s="19" t="s">
         <v>34</v>
       </c>
@@ -1667,13 +1671,13 @@
       </c>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="2:12" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="38.25" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="43"/>
-      <c r="E25" s="44"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="19" t="s">
         <v>35</v>
       </c>
@@ -1685,7 +1689,7 @@
       </c>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
       <c r="C26" s="21"/>
       <c r="D26" s="23"/>
@@ -1697,13 +1701,13 @@
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="44"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="40"/>
       <c r="F27" s="37">
         <f>SUM(F23:F25)</f>
         <v>0</v>
@@ -1718,7 +1722,7 @@
       </c>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -1728,7 +1732,7 @@
       <c r="H28" s="17"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -1738,7 +1742,7 @@
       <c r="H29" s="11"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -1748,7 +1752,7 @@
       <c r="H30" s="11"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="6"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
@@ -1758,7 +1762,7 @@
       <c r="H31" s="11"/>
       <c r="I31" s="12"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="6"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -1768,7 +1772,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="12"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33" s="6"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
@@ -1778,7 +1782,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34" s="6"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -1788,7 +1792,7 @@
       <c r="H34" s="11"/>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="6"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -1798,7 +1802,7 @@
       <c r="H35" s="11"/>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36" s="6"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -1808,7 +1812,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="12"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37" s="6"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -1818,7 +1822,7 @@
       <c r="H37" s="11"/>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38" s="6"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -1828,7 +1832,7 @@
       <c r="H38" s="11"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39" s="6"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -1838,7 +1842,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="12"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B40" s="6"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1848,7 +1852,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="12"/>
     </row>
-    <row r="41" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="6"/>
       <c r="C41" s="26" t="s">
         <v>5</v>
@@ -1860,13 +1864,13 @@
       <c r="F41" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="49" t="s">
+      <c r="G41" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="H41" s="49"/>
+      <c r="H41" s="41"/>
       <c r="I41" s="27"/>
     </row>
-    <row r="42" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="6"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
@@ -1880,7 +1884,7 @@
       <c r="H42" s="36"/>
       <c r="I42" s="27"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" s="6"/>
       <c r="D43" s="26"/>
       <c r="F43" s="26" t="s">
@@ -1893,7 +1897,7 @@
       <c r="I43" s="27"/>
       <c r="J43" s="26"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" s="6"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
@@ -1908,7 +1912,7 @@
       <c r="I44" s="27"/>
       <c r="J44" s="26"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45" s="6"/>
       <c r="C45" s="36" t="s">
         <v>28</v>
@@ -1921,7 +1925,7 @@
       <c r="I45" s="29"/>
       <c r="J45" s="30"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B46" s="31"/>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
@@ -1933,11 +1937,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="G41:H41"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C20:E20"/>
@@ -1947,6 +1946,11 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="G41:H41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
100878 Adult Funding Claim - corrected header alignment issues
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/AdultFundingClaimReportTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E294766-1697-4FC1-96C1-E6AE409A960A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857233CC-83E9-438C-862A-979AE8178D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,6 +556,18 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
@@ -568,32 +580,20 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1297,7 +1297,7 @@
   <dimension ref="B2:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1305,9 +1305,10 @@
     <col min="1" max="1" width="3.1328125" style="5" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="22.86328125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="34" style="5" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="15.53125" style="5" customWidth="1"/>
-    <col min="6" max="8" width="20.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="22.73046875" style="5" customWidth="1"/>
+    <col min="7" max="8" width="22.6640625" style="5" customWidth="1"/>
     <col min="9" max="9" width="4.1328125" style="5" customWidth="1"/>
     <col min="10" max="10" width="2.33203125" style="5" customWidth="1"/>
     <col min="11" max="16384" width="9.1328125" style="5"/>
@@ -1330,11 +1331,11 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -1456,14 +1457,14 @@
     </row>
     <row r="12" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
       <c r="I12" s="12"/>
     </row>
     <row r="13" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1478,11 +1479,11 @@
     </row>
     <row r="14" spans="2:12" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="48"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="47"/>
       <c r="F14" s="18" t="s">
         <v>9</v>
       </c>
@@ -1496,11 +1497,11 @@
     </row>
     <row r="15" spans="2:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="19" t="s">
         <v>29</v>
       </c>
@@ -1516,11 +1517,11 @@
     </row>
     <row r="16" spans="2:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="40"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="19" t="s">
         <v>30</v>
       </c>
@@ -1536,11 +1537,11 @@
     </row>
     <row r="17" spans="2:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="40"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="19" t="s">
         <v>31</v>
       </c>
@@ -1556,11 +1557,11 @@
     </row>
     <row r="18" spans="2:12" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="19" t="s">
         <v>32</v>
       </c>
@@ -1588,11 +1589,11 @@
     </row>
     <row r="20" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="39"/>
-      <c r="E20" s="40"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="37">
         <f>SUM(F15:F18)</f>
         <v>0</v>
@@ -1619,11 +1620,11 @@
     </row>
     <row r="22" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="45"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="18" t="s">
         <v>9</v>
       </c>
@@ -1637,11 +1638,11 @@
     </row>
     <row r="23" spans="2:12" ht="38.25" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="19" t="s">
         <v>33</v>
       </c>
@@ -1655,11 +1656,11 @@
     </row>
     <row r="24" spans="2:12" ht="38.25" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="39"/>
-      <c r="E24" s="40"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="19" t="s">
         <v>34</v>
       </c>
@@ -1673,11 +1674,11 @@
     </row>
     <row r="25" spans="2:12" ht="38.25" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="40"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="44"/>
       <c r="F25" s="19" t="s">
         <v>35</v>
       </c>
@@ -1703,11 +1704,11 @@
     </row>
     <row r="27" spans="2:12" ht="13.15" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
-      <c r="C27" s="38" t="s">
+      <c r="C27" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="44"/>
       <c r="F27" s="37">
         <f>SUM(F23:F25)</f>
         <v>0</v>
@@ -1864,10 +1865,10 @@
       <c r="F41" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="41" t="s">
+      <c r="G41" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H41" s="41"/>
+      <c r="H41" s="49"/>
       <c r="I41" s="27"/>
     </row>
     <row r="42" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1937,6 +1938,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="G41:H41"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C20:E20"/>
@@ -1946,11 +1952,6 @@
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="G41:H41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" r:id="rId1"/>

</xml_diff>